<commit_message>
Updated spreadsheets with submitted info
</commit_message>
<xml_diff>
--- a/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_HUD_2020.xlsx
+++ b/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_HUD_2020.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Global_Decisions--&gt;" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t xml:space="preserve">Flags</t>
   </si>
@@ -174,6 +174,9 @@
     <t xml:space="preserve">Include station labels on trend maps?</t>
   </si>
   <si>
+    <t xml:space="preserve">Convert wind speeds from m/s to mph?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parameter</t>
   </si>
   <si>
@@ -189,6 +192,9 @@
     <t xml:space="preserve">WQ_Threshold</t>
   </si>
   <si>
+    <t xml:space="preserve">Free_Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">temp</t>
   </si>
   <si>
@@ -348,28 +354,10 @@
     <t xml:space="preserve">&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">2000</t>
   </si>
   <si>
     <t xml:space="preserve">2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convert winds from m/s to mph?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free_Y</t>
   </si>
 </sst>
 </file>
@@ -785,7 +773,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>
@@ -803,7 +791,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10" outlineLevelCol="1"/>
@@ -813,51 +801,51 @@
     <col min="6" max="6" width="22.01" hidden="false" outlineLevel="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" ht="13.8" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" ht="13.8" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" ht="13.8" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1">
+    </row>
+    <row r="4" ht="13.8" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -866,172 +854,172 @@
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" ht="13.8" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" ht="13.8" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" ht="13.8" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" ht="13.8" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" ht="13.8" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" ht="13.8" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1">
+    </row>
+    <row r="11" ht="13.8" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" ht="13.8" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" ht="15" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" ht="13.8" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" ht="13.8" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" ht="15" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" ht="13.8" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1">
+    <row r="16" ht="13.8" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" ht="13.8" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1">
+    </row>
+    <row r="18" ht="13.8" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" ht="15" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" ht="13.8" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" ht="15" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" ht="13.8" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1">
+    <row r="21" ht="13.8" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1">
+    <row r="22" ht="13.8" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>0.1</v>
@@ -1039,7 +1027,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>
@@ -1057,7 +1045,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
@@ -1068,18 +1056,18 @@
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>108</v>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>109</v>
+      <c r="A3" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>110</v>
+      <c r="A4" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -1087,14 +1075,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>111</v>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>
@@ -1112,7 +1100,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10" outlineLevelCol="1"/>
@@ -1130,7 +1118,7 @@
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>2020</v>
@@ -1138,13 +1126,13 @@
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>
@@ -1161,7 +1149,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1174,12 +1162,10 @@
     <col min="5" max="5" width="12.86" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="6" max="6" width="15.71" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="7" max="7" width="16.14" hidden="false" outlineLevel="1" customWidth="1"/>
-    <col min="8" max="8" width="8.41" hidden="false" outlineLevel="1" customWidth="1"/>
-    <col min="9" max="9" width="8.41" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="10" max="10" width="10.85" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="11" max="11" width="8.14" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="12" max="12" width="10.42" hidden="false" outlineLevel="1" customWidth="1"/>
-    <col min="13" max="13" width="10.13" hidden="false" outlineLevel="1" customWidth="1"/>
+    <col min="13" max="13" width="10.12" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="14" max="14" width="12.42" hidden="false" outlineLevel="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1384,7 +1370,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>
@@ -1401,15 +1387,15 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="13.86" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="2" max="2" width="13.86" hidden="false" outlineLevel="1" customWidth="1"/>
-    <col min="3" max="3" width="18.13" hidden="false" outlineLevel="1" customWidth="1"/>
+    <col min="3" max="3" width="18.12" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="4" max="4" width="18.29" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="5" max="5" width="18.71" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="6" max="6" width="18.71" hidden="false" outlineLevel="1" customWidth="1"/>
@@ -1440,7 +1426,7 @@
         <v>-74.7192</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>-74.3967</v>
+        <v>-74.5044</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
@@ -1460,7 +1446,7 @@
         <v>41.0497</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>41.2906</v>
+        <v>41.2104</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>34</v>
@@ -1478,7 +1464,7 @@
         <v>-72.9879</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>-73.3164</v>
+        <v>-73.2071</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>35</v>
@@ -1496,7 +1482,7 @@
         <v>42.3282</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>42.0884</v>
+        <v>42.1683</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>34</v>
@@ -1515,27 +1501,13 @@
       <c r="C6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D6"/>
       <c r="E6"/>
-      <c r="F6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
+      <c r="F6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>
@@ -1553,7 +1525,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10" outlineLevelCol="1"/>
@@ -1649,17 +1621,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" ht="13.8" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>
@@ -1684,7 +1656,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>
@@ -1701,8 +1673,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10" outlineLevelCol="1"/>
@@ -1712,75 +1684,73 @@
     <col min="3" max="3" width="15.71" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="4" max="4" width="15.71" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="5" max="5" width="13.43" hidden="false" outlineLevel="1" customWidth="1"/>
-    <col min="6" max="6" width="31.86" hidden="false" outlineLevel="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44" hidden="false" outlineLevel="1" customWidth="1"/>
     <col min="7" max="7" width="28.98" hidden="false" outlineLevel="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" ht="13.8" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" ht="13.8" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E2"/>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" ht="13.8" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E3"/>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" ht="13.8" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>48</v>
@@ -1788,337 +1758,319 @@
       <c r="E4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" ht="13.8" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E5"/>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" ht="13.8" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E6"/>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" ht="13.8" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E7"/>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
+      <c r="F7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" ht="13.8" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8"/>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" ht="13.8" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9"/>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" ht="13.8" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E10"/>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" ht="13.8" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E11"/>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1">
+      <c r="F11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" ht="13.8" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E12"/>
-      <c r="F12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" ht="15" customHeight="1">
+      <c r="F12" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" ht="13.8" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13"/>
-      <c r="F13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1">
+      <c r="F13" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" ht="13.8" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E14"/>
-      <c r="F14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" ht="15" customHeight="1">
+      <c r="F14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" ht="13.8" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E15"/>
-      <c r="F15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" ht="15" customHeight="1">
+      <c r="F15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" ht="13.8" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E16"/>
-      <c r="F16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1">
+      <c r="F16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" ht="13.8" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E17"/>
-      <c r="F17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1">
+      <c r="F17" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" ht="13.8" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E18"/>
-      <c r="F18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" ht="15" customHeight="1">
+      <c r="F18" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" ht="13.8" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E19"/>
-      <c r="F19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" ht="15" customHeight="1">
+      <c r="F19" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" ht="13.8" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E20"/>
-      <c r="F20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" ht="15" customHeight="1">
+      <c r="F20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" ht="13.8" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E21"/>
-      <c r="F21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" ht="15" customHeight="1">
+      <c r="F21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" ht="13.8" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E22"/>
-      <c r="F22" t="s">
-        <v>39</v>
+      <c r="F22" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>
@@ -2135,8 +2087,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10" outlineLevelCol="1"/>
@@ -2155,59 +2107,59 @@
     <col min="14" max="14" width="10" hidden="false" outlineLevel="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" ht="13.8" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" ht="13.8" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0.05</v>
@@ -2219,15 +2171,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" ht="13.8" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.05</v>
@@ -2239,15 +2191,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" ht="13.8" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -2256,22 +2208,22 @@
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>39</v>
@@ -2280,15 +2232,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" ht="13.8" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0.05</v>
@@ -2300,15 +2252,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" ht="13.8" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>0.9</v>
@@ -2317,15 +2269,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" ht="13.8" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0.05</v>
@@ -2337,15 +2289,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" ht="13.8" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0.05</v>
@@ -2357,15 +2309,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" ht="13.8" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0.05</v>
@@ -2377,15 +2329,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" ht="13.8" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0.05</v>
@@ -2397,15 +2349,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" ht="13.8" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0.05</v>
@@ -2417,15 +2369,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" ht="13.8" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0.05</v>
@@ -2437,84 +2389,84 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1">
+    <row r="13" ht="13.8" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1">
+    <row r="14" ht="13.8" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1">
+    <row r="15" ht="13.8" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.01</v>
+        <v>0.07</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>0.015</v>
+        <v>0.1</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="I15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.015</v>
-      </c>
-    </row>
-    <row r="16" ht="15" customHeight="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" ht="13.8" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0.05</v>
@@ -2526,15 +2478,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1">
+    <row r="17" ht="13.8" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0.05</v>
@@ -2546,15 +2498,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" ht="13.8" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>0.05</v>
@@ -2566,15 +2518,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" ht="15" customHeight="1">
+    <row r="19" ht="13.8" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>0.05</v>
@@ -2586,111 +2538,132 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1">
+    <row r="20" ht="13.8" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="I20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" ht="15" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" ht="13.8" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" ht="15" customHeight="1">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" ht="13.8" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0.01</v>
+        <v>0.07</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>0.015</v>
+        <v>0.1</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="I22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M22" s="1" t="n">
-        <v>0.015</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader/>
     <oddFooter/>

</xml_diff>